<commit_message>
Faculty edit settings for Faculty User Login
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data1.xlsx
+++ b/src/main/resources/UMS_Data1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="190">
   <si>
     <t>Course Code</t>
   </si>
@@ -63,372 +63,372 @@
     <t>Room 101</t>
   </si>
   <si>
+    <t>Dr. Alan Turing</t>
+  </si>
+  <si>
+    <t>Literature Basics</t>
+  </si>
+  <si>
+    <t>ENG101</t>
+  </si>
+  <si>
+    <t>Tue/Thu 10-12 PM</t>
+  </si>
+  <si>
+    <t>12/16/2025 10:00</t>
+  </si>
+  <si>
+    <t>Room 102</t>
+  </si>
+  <si>
+    <t>Prof. Emily Brontë</t>
+  </si>
+  <si>
+    <t>Section 2</t>
+  </si>
+  <si>
+    <t>Mon/Wed 10-12 PM</t>
+  </si>
+  <si>
+    <t>Introduction to Programming</t>
+  </si>
+  <si>
+    <t>CS201</t>
+  </si>
+  <si>
+    <t>Tue/Thu 12-2 PM</t>
+  </si>
+  <si>
+    <t>12/16/2025 12:30</t>
+  </si>
+  <si>
+    <t>Room 103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prof. Bahar Nozari </t>
+  </si>
+  <si>
+    <t>Introduction to Chemistry</t>
+  </si>
+  <si>
+    <t>CHEM200</t>
+  </si>
+  <si>
+    <t>Mon/ Thu 3-4 PM</t>
+  </si>
+  <si>
+    <t>12/14/2025 04:00</t>
+  </si>
+  <si>
+    <t>Room 201</t>
+  </si>
+  <si>
+    <t>Dr. Lucka Lucku</t>
+  </si>
+  <si>
+    <t>Mon/ Tue 5-6 PM</t>
+  </si>
+  <si>
+    <t>Section 3</t>
+  </si>
+  <si>
+    <t>Fri/ Thu 2-3 PM</t>
+  </si>
+  <si>
+    <t>Introduction to French</t>
+  </si>
+  <si>
+    <t>Tue/Thur 4:30 - 5:30 PM</t>
+  </si>
+  <si>
+    <t>12/13/2025 10:00</t>
+  </si>
+  <si>
+    <t>Room 202</t>
+  </si>
+  <si>
+    <t>Dr. Lakyn Copeland</t>
+  </si>
+  <si>
+    <t>Tue/Thur 5:30 - 6:30 PM</t>
+  </si>
+  <si>
+    <t>Water Resources</t>
+  </si>
+  <si>
+    <t>ENGG402</t>
+  </si>
+  <si>
+    <t>Mon/Fri 9:00 - 10:30</t>
+  </si>
+  <si>
+    <t>12/01/2025 09:00</t>
+  </si>
+  <si>
+    <t>Room 203</t>
+  </si>
+  <si>
+    <t>Dr. Albozr Gharabaghi</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Academic Level</t>
+  </si>
+  <si>
+    <t>Current Semester</t>
+  </si>
+  <si>
+    <t>Profile Picture</t>
+  </si>
+  <si>
+    <t>Registered Subjects</t>
+  </si>
+  <si>
+    <t>Thesis Title</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>S20250001</t>
+  </si>
+  <si>
+    <t>Alice Smith</t>
+  </si>
+  <si>
+    <t>123 Maple St.</t>
+  </si>
+  <si>
+    <t>555-1234</t>
+  </si>
+  <si>
+    <t>alice@example.edu</t>
+  </si>
+  <si>
+    <t>Undergraduate</t>
+  </si>
+  <si>
+    <t>Fall 2025</t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>default123</t>
+  </si>
+  <si>
+    <t>S20250002</t>
+  </si>
+  <si>
+    <t>Bob Johnson</t>
+  </si>
+  <si>
+    <t>456 Oak St.</t>
+  </si>
+  <si>
+    <t>555-5678</t>
+  </si>
+  <si>
+    <t>bob@example.edu</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>"The detection of oil under ice by remote mode conversion of ultrasound"</t>
+  </si>
+  <si>
+    <t>S20250003</t>
+  </si>
+  <si>
+    <t>Carol Williams</t>
+  </si>
+  <si>
+    <t>789 Pine St.</t>
+  </si>
+  <si>
+    <t>555-9012</t>
+  </si>
+  <si>
+    <t>carol@example.edu</t>
+  </si>
+  <si>
+    <t>ENGG402, HIST101</t>
+  </si>
+  <si>
+    <t>"On the economic optimality of marine reserves when fishing damages habitat"</t>
+  </si>
+  <si>
+    <t>S20250004</t>
+  </si>
+  <si>
+    <t>Lucka Racki</t>
+  </si>
+  <si>
+    <t>1767 Jane St.</t>
+  </si>
+  <si>
+    <t>439-9966</t>
+  </si>
+  <si>
+    <t>lucka@example.edu</t>
+  </si>
+  <si>
+    <t>Bio300</t>
+  </si>
+  <si>
+    <t>S20250005</t>
+  </si>
+  <si>
+    <t>David Lee</t>
+  </si>
+  <si>
+    <t>90 Elm St.</t>
+  </si>
+  <si>
+    <t>555-3456</t>
+  </si>
+  <si>
+    <t>lee@example.edu</t>
+  </si>
+  <si>
+    <t>HIST101</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>S20250006</t>
+  </si>
+  <si>
+    <t>Emily Brown</t>
+  </si>
+  <si>
+    <t>111 Oak Ave.</t>
+  </si>
+  <si>
+    <t>555-7890</t>
+  </si>
+  <si>
+    <t>brown@example.edu</t>
+  </si>
+  <si>
+    <t>Chem200</t>
+  </si>
+  <si>
+    <t>Synthesis and Characterization of Novel Catalysts</t>
+  </si>
+  <si>
+    <t>S20250007</t>
+  </si>
+  <si>
+    <t>George Smith</t>
+  </si>
+  <si>
+    <t>222 Pine Rd.</t>
+  </si>
+  <si>
+    <t>555-2345</t>
+  </si>
+  <si>
+    <t>smith@example.edu</t>
+  </si>
+  <si>
+    <t>Music102</t>
+  </si>
+  <si>
+    <t>S20250008</t>
+  </si>
+  <si>
+    <t>Helen Jones</t>
+  </si>
+  <si>
+    <t>333 Maple Dr.</t>
+  </si>
+  <si>
+    <t>555-4567</t>
+  </si>
+  <si>
+    <t>jones@example.edu</t>
+  </si>
+  <si>
+    <t>PSYCHO100, Music102, HIST101</t>
+  </si>
+  <si>
+    <t>The Effects of Stress on Cognitive Function</t>
+  </si>
+  <si>
+    <t>S20250009</t>
+  </si>
+  <si>
+    <t>Isaac Clark</t>
+  </si>
+  <si>
+    <t>444 Cedar Ln.</t>
+  </si>
+  <si>
+    <t>555-8901</t>
+  </si>
+  <si>
+    <t>clark@example.edu</t>
+  </si>
+  <si>
+    <t>BIo300</t>
+  </si>
+  <si>
+    <t>S20250010</t>
+  </si>
+  <si>
+    <t>Jennifer Davis</t>
+  </si>
+  <si>
+    <t>555 Oakwood Pl.</t>
+  </si>
+  <si>
+    <t>davis@example.edu</t>
+  </si>
+  <si>
+    <t>The Renaissance: Art, Culture, and Society</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Research Interest</t>
+  </si>
+  <si>
+    <t>Office Location</t>
+  </si>
+  <si>
+    <t>Courses Offered</t>
+  </si>
+  <si>
     <t>F0001</t>
   </si>
   <si>
-    <t>Literature Basics</t>
-  </si>
-  <si>
-    <t>ENG101</t>
-  </si>
-  <si>
-    <t>Section 2</t>
-  </si>
-  <si>
-    <t>Tue/Thu 10-12 PM</t>
-  </si>
-  <si>
-    <t>12/16/2025 10:00</t>
-  </si>
-  <si>
-    <t>Room 102</t>
-  </si>
-  <si>
-    <t>Unassigned</t>
-  </si>
-  <si>
-    <t>Mon/Wed 10-12 PM</t>
-  </si>
-  <si>
-    <t>Introduction to Programming</t>
-  </si>
-  <si>
-    <t>CS201</t>
-  </si>
-  <si>
-    <t>Tue/Thu 12-2 PM</t>
-  </si>
-  <si>
-    <t>12/16/2025 12:30</t>
-  </si>
-  <si>
-    <t>Room 103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prof. Bahar Nozari </t>
-  </si>
-  <si>
-    <t>Introduction to Chemistry</t>
-  </si>
-  <si>
-    <t>CHEM200</t>
-  </si>
-  <si>
-    <t>Mon/ Thu 3-4 PM</t>
-  </si>
-  <si>
-    <t>12/14/2025 04:00</t>
-  </si>
-  <si>
-    <t>Room 201</t>
-  </si>
-  <si>
-    <t>Dr. Lucka Lucku</t>
-  </si>
-  <si>
-    <t>Mon/ Tue 5-6 PM</t>
-  </si>
-  <si>
-    <t>Section 3</t>
-  </si>
-  <si>
-    <t>Fri/ Thu 2-3 PM</t>
-  </si>
-  <si>
-    <t>Introduction to French</t>
-  </si>
-  <si>
-    <t>Tue/Thur 4:30 - 5:30 PM</t>
-  </si>
-  <si>
-    <t>12/13/2025 10:00</t>
-  </si>
-  <si>
-    <t>Room 202</t>
-  </si>
-  <si>
-    <t>Dr. Lakyn Copeland</t>
-  </si>
-  <si>
-    <t>Tue/Thur 5:30 - 6:30 PM</t>
-  </si>
-  <si>
-    <t>Water Resources</t>
-  </si>
-  <si>
-    <t>ENGG402</t>
-  </si>
-  <si>
-    <t>Mon/Fri 9:00 - 10:30</t>
-  </si>
-  <si>
-    <t>12/01/2025 09:00</t>
-  </si>
-  <si>
-    <t>Room 203</t>
-  </si>
-  <si>
-    <t>Dr. Albozr Gharabaghi</t>
-  </si>
-  <si>
-    <t>Student ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Academic Level</t>
-  </si>
-  <si>
-    <t>Current Semester</t>
-  </si>
-  <si>
-    <t>Profile Picture</t>
-  </si>
-  <si>
-    <t>Registered Subjects</t>
-  </si>
-  <si>
-    <t>Thesis Title</t>
-  </si>
-  <si>
-    <t>Progress</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>S20250001</t>
-  </si>
-  <si>
-    <t>Alice Smith</t>
-  </si>
-  <si>
-    <t>123 Maple St.</t>
-  </si>
-  <si>
-    <t>555-1234</t>
-  </si>
-  <si>
-    <t>alice@example.edu</t>
-  </si>
-  <si>
-    <t>Undergraduate</t>
-  </si>
-  <si>
-    <t>Fall 2025</t>
-  </si>
-  <si>
-    <t>custom</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>default123</t>
-  </si>
-  <si>
-    <t>S20250002</t>
-  </si>
-  <si>
-    <t>Bob Johnson</t>
-  </si>
-  <si>
-    <t>456 Oak St.</t>
-  </si>
-  <si>
-    <t>555-5678</t>
-  </si>
-  <si>
-    <t>bob@example.edu</t>
-  </si>
-  <si>
-    <t>Graduate</t>
-  </si>
-  <si>
-    <t>"The detection of oil under ice by remote mode conversion of ultrasound"</t>
-  </si>
-  <si>
-    <t>S20250003</t>
-  </si>
-  <si>
-    <t>Carol Williams</t>
-  </si>
-  <si>
-    <t>789 Pine St.</t>
-  </si>
-  <si>
-    <t>555-9012</t>
-  </si>
-  <si>
-    <t>carol@example.edu</t>
-  </si>
-  <si>
-    <t>ENGG402, HIST101</t>
-  </si>
-  <si>
-    <t>"On the economic optimality of marine reserves when fishing damages habitat"</t>
-  </si>
-  <si>
-    <t>S20250004</t>
-  </si>
-  <si>
-    <t>Lucka Racki</t>
-  </si>
-  <si>
-    <t>1767 Jane St.</t>
-  </si>
-  <si>
-    <t>439-9966</t>
-  </si>
-  <si>
-    <t>lucka@example.edu</t>
-  </si>
-  <si>
-    <t>Bio300</t>
-  </si>
-  <si>
-    <t>S20250005</t>
-  </si>
-  <si>
-    <t>David Lee</t>
-  </si>
-  <si>
-    <t>90 Elm St.</t>
-  </si>
-  <si>
-    <t>555-3456</t>
-  </si>
-  <si>
-    <t>lee@example.edu</t>
-  </si>
-  <si>
-    <t>HIST101</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>S20250006</t>
-  </si>
-  <si>
-    <t>Emily Brown</t>
-  </si>
-  <si>
-    <t>111 Oak Ave.</t>
-  </si>
-  <si>
-    <t>555-7890</t>
-  </si>
-  <si>
-    <t>brown@example.edu</t>
-  </si>
-  <si>
-    <t>Chem200</t>
-  </si>
-  <si>
-    <t>Synthesis and Characterization of Novel Catalysts</t>
-  </si>
-  <si>
-    <t>S20250007</t>
-  </si>
-  <si>
-    <t>George Smith</t>
-  </si>
-  <si>
-    <t>222 Pine Rd.</t>
-  </si>
-  <si>
-    <t>555-2345</t>
-  </si>
-  <si>
-    <t>smith@example.edu</t>
-  </si>
-  <si>
-    <t>Music102</t>
-  </si>
-  <si>
-    <t>S20250008</t>
-  </si>
-  <si>
-    <t>Helen Jones</t>
-  </si>
-  <si>
-    <t>333 Maple Dr.</t>
-  </si>
-  <si>
-    <t>555-4567</t>
-  </si>
-  <si>
-    <t>jones@example.edu</t>
-  </si>
-  <si>
-    <t>PSYCHO100, Music102, HIST101</t>
-  </si>
-  <si>
-    <t>The Effects of Stress on Cognitive Function</t>
-  </si>
-  <si>
-    <t>S20250009</t>
-  </si>
-  <si>
-    <t>Isaac Clark</t>
-  </si>
-  <si>
-    <t>444 Cedar Ln.</t>
-  </si>
-  <si>
-    <t>555-8901</t>
-  </si>
-  <si>
-    <t>clark@example.edu</t>
-  </si>
-  <si>
-    <t>BIo300</t>
-  </si>
-  <si>
-    <t>S20250010</t>
-  </si>
-  <si>
-    <t>Jennifer Davis</t>
-  </si>
-  <si>
-    <t>555 Oakwood Pl.</t>
-  </si>
-  <si>
-    <t>davis@example.edu</t>
-  </si>
-  <si>
-    <t>The Renaissance: Art, Culture, and Society</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Degree</t>
-  </si>
-  <si>
-    <t>Research Interest</t>
-  </si>
-  <si>
-    <t>Office Location</t>
-  </si>
-  <si>
-    <t>Courses Offered</t>
-  </si>
-  <si>
-    <t>Dr. Alan Turing</t>
-  </si>
-  <si>
     <t>Ph.D.</t>
   </si>
   <si>
@@ -439,9 +439,6 @@
   </si>
   <si>
     <t>F0002</t>
-  </si>
-  <si>
-    <t>Prof. Emily Brontë</t>
   </si>
   <si>
     <t>Master's</t>
@@ -948,22 +945,22 @@
         <v>17</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E3" t="n" s="0">
         <v>25.0</v>
       </c>
       <c r="F3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="H3" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="I3" t="s" s="0">
         <v>21</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -977,7 +974,7 @@
         <v>17</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E4" t="n" s="0">
         <v>25.0</v>
@@ -986,13 +983,13 @@
         <v>23</v>
       </c>
       <c r="G4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="I4" t="s" s="0">
         <v>21</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -1064,7 +1061,7 @@
         <v>31</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E7" t="n" s="0">
         <v>50.0</v>
@@ -1151,7 +1148,7 @@
         <v>17</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E10" t="n" s="0">
         <v>25.0</v>
@@ -1670,10 +1667,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>15</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>136</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>137</v>
@@ -1685,7 +1682,7 @@
         <v>139</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>9</v>
@@ -1699,16 +1696,16 @@
         <v>140</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="D3" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="E3" t="s" s="0">
         <v>143</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>144</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>42</v>
@@ -1722,25 +1719,25 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>145</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>146</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>137</v>
       </c>
       <c r="D4" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="F4" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="G4" t="s" s="0">
         <v>149</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>150</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>72</v>
@@ -1748,19 +1745,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>43</v>
       </c>
       <c r="C5" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>143</v>
-      </c>
       <c r="E5" t="s" s="0">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>34</v>
@@ -1774,22 +1771,22 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>153</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>154</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>137</v>
       </c>
       <c r="D6" t="s" s="0">
+        <v>154</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="F6" t="s" s="0">
         <v>156</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>157</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>45</v>
@@ -1816,7 +1813,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s" s="31">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2">
@@ -1824,7 +1821,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3">
@@ -1832,7 +1829,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4">
@@ -1840,7 +1837,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5">
@@ -1848,15 +1845,15 @@
         <v>31</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>163</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>164</v>
       </c>
     </row>
     <row r="7">
@@ -1864,7 +1861,7 @@
         <v>46</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8">
@@ -1872,23 +1869,23 @@
         <v>98</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="B9" t="s" s="0">
         <v>167</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>168</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="B10" t="s" s="0">
         <v>169</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1906,89 +1903,89 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="32">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s" s="33">
         <v>52</v>
       </c>
       <c r="C1" t="s" s="34">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s" s="35">
         <v>7</v>
       </c>
       <c r="E1" t="s" s="36">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F1" t="s" s="37">
         <v>4</v>
       </c>
       <c r="G1" t="s" s="38">
+        <v>173</v>
+      </c>
+      <c r="H1" t="s" s="39">
         <v>174</v>
       </c>
-      <c r="H1" t="s" s="39">
+      <c r="I1" t="s" s="40">
         <v>175</v>
-      </c>
-      <c r="I1" t="s" s="40">
-        <v>176</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="D2" t="s" s="0">
         <v>179</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="E2" t="s" s="0">
         <v>180</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>181</v>
       </c>
       <c r="F2" t="n" s="0">
         <v>100.0</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>70</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>184</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s" s="0">
         <v>185</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="D3" t="s" s="0">
         <v>186</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="E3" t="s" s="0">
         <v>187</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>188</v>
       </c>
       <c r="F3" t="n" s="0">
         <v>50.0</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>70</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated event admin controller for image browsing and displaying.
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data1.xlsx
+++ b/src/main/resources/UMS_Data1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="197">
   <si>
     <t>Course Code</t>
   </si>
@@ -63,372 +63,372 @@
     <t>Room 101</t>
   </si>
   <si>
+    <t>Dr. Alan Turing</t>
+  </si>
+  <si>
+    <t>Literature Basics</t>
+  </si>
+  <si>
+    <t>ENG101</t>
+  </si>
+  <si>
+    <t>Tue/Thu 10-12 PM</t>
+  </si>
+  <si>
+    <t>12/16/2025 10:00</t>
+  </si>
+  <si>
+    <t>Room 102</t>
+  </si>
+  <si>
+    <t>Prof. Emily Brontë</t>
+  </si>
+  <si>
+    <t>Section 2</t>
+  </si>
+  <si>
+    <t>Mon/Wed 10-12 PM</t>
+  </si>
+  <si>
+    <t>Introduction to Programming</t>
+  </si>
+  <si>
+    <t>CS201</t>
+  </si>
+  <si>
+    <t>Tue/Thu 12-2 PM</t>
+  </si>
+  <si>
+    <t>12/16/2025 12:30</t>
+  </si>
+  <si>
+    <t>Room 103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prof. Bahar Nozari </t>
+  </si>
+  <si>
+    <t>Introduction to Chemistry</t>
+  </si>
+  <si>
+    <t>CHEM200</t>
+  </si>
+  <si>
+    <t>Mon/ Thu 3-4 PM</t>
+  </si>
+  <si>
+    <t>12/14/2025 04:00</t>
+  </si>
+  <si>
+    <t>Room 201</t>
+  </si>
+  <si>
+    <t>Dr. Lucka Lucku</t>
+  </si>
+  <si>
+    <t>Mon/ Tue 5-6 PM</t>
+  </si>
+  <si>
+    <t>Section 3</t>
+  </si>
+  <si>
+    <t>Fri/ Thu 2-3 PM</t>
+  </si>
+  <si>
+    <t>Introduction to French</t>
+  </si>
+  <si>
+    <t>Tue/Thur 4:30 - 5:30 PM</t>
+  </si>
+  <si>
+    <t>12/13/2025 10:00</t>
+  </si>
+  <si>
+    <t>Room 202</t>
+  </si>
+  <si>
+    <t>Dr. Lakyn Copeland</t>
+  </si>
+  <si>
+    <t>Tue/Thur 5:30 - 6:30 PM</t>
+  </si>
+  <si>
+    <t>Water Resources</t>
+  </si>
+  <si>
+    <t>ENGG402</t>
+  </si>
+  <si>
+    <t>Mon/Fri 9:00 - 10:30</t>
+  </si>
+  <si>
+    <t>12/01/2025 09:00</t>
+  </si>
+  <si>
+    <t>Room 203</t>
+  </si>
+  <si>
+    <t>Dr. Albozr Gharabaghi</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Academic Level</t>
+  </si>
+  <si>
+    <t>Current Semester</t>
+  </si>
+  <si>
+    <t>Profile Picture</t>
+  </si>
+  <si>
+    <t>Registered Subjects</t>
+  </si>
+  <si>
+    <t>Thesis Title</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>S20250001</t>
+  </si>
+  <si>
+    <t>Alice Smith</t>
+  </si>
+  <si>
+    <t>123 Maple St.</t>
+  </si>
+  <si>
+    <t>555-1234</t>
+  </si>
+  <si>
+    <t>alice@example.edu</t>
+  </si>
+  <si>
+    <t>Undergraduate</t>
+  </si>
+  <si>
+    <t>Fall 2025</t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>default123</t>
+  </si>
+  <si>
+    <t>S20250002</t>
+  </si>
+  <si>
+    <t>Bob Johnson</t>
+  </si>
+  <si>
+    <t>456 Oak St.</t>
+  </si>
+  <si>
+    <t>555-5678</t>
+  </si>
+  <si>
+    <t>bob@example.edu</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>"The detection of oil under ice by remote mode conversion of ultrasound"</t>
+  </si>
+  <si>
+    <t>S20250003</t>
+  </si>
+  <si>
+    <t>Carol Williams</t>
+  </si>
+  <si>
+    <t>789 Pine St.</t>
+  </si>
+  <si>
+    <t>555-9012</t>
+  </si>
+  <si>
+    <t>carol@example.edu</t>
+  </si>
+  <si>
+    <t>ENGG402, HIST101</t>
+  </si>
+  <si>
+    <t>"On the economic optimality of marine reserves when fishing damages habitat"</t>
+  </si>
+  <si>
+    <t>S20250004</t>
+  </si>
+  <si>
+    <t>Lucka Racki</t>
+  </si>
+  <si>
+    <t>1767 Jane St.</t>
+  </si>
+  <si>
+    <t>439-9966</t>
+  </si>
+  <si>
+    <t>lucka@example.edu</t>
+  </si>
+  <si>
+    <t>Bio300</t>
+  </si>
+  <si>
+    <t>S20250005</t>
+  </si>
+  <si>
+    <t>David Lee</t>
+  </si>
+  <si>
+    <t>90 Elm St.</t>
+  </si>
+  <si>
+    <t>555-3456</t>
+  </si>
+  <si>
+    <t>lee@example.edu</t>
+  </si>
+  <si>
+    <t>HIST101</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>S20250006</t>
+  </si>
+  <si>
+    <t>Emily Brown</t>
+  </si>
+  <si>
+    <t>111 Oak Ave.</t>
+  </si>
+  <si>
+    <t>555-7890</t>
+  </si>
+  <si>
+    <t>brown@example.edu</t>
+  </si>
+  <si>
+    <t>Chem200</t>
+  </si>
+  <si>
+    <t>Synthesis and Characterization of Novel Catalysts</t>
+  </si>
+  <si>
+    <t>S20250007</t>
+  </si>
+  <si>
+    <t>George Smith</t>
+  </si>
+  <si>
+    <t>222 Pine Rd.</t>
+  </si>
+  <si>
+    <t>555-2345</t>
+  </si>
+  <si>
+    <t>smith@example.edu</t>
+  </si>
+  <si>
+    <t>Music102</t>
+  </si>
+  <si>
+    <t>S20250008</t>
+  </si>
+  <si>
+    <t>Helen Jones</t>
+  </si>
+  <si>
+    <t>333 Maple Dr.</t>
+  </si>
+  <si>
+    <t>555-4567</t>
+  </si>
+  <si>
+    <t>jones@example.edu</t>
+  </si>
+  <si>
+    <t>PSYCHO100, Music102, HIST101</t>
+  </si>
+  <si>
+    <t>The Effects of Stress on Cognitive Function</t>
+  </si>
+  <si>
+    <t>S20250009</t>
+  </si>
+  <si>
+    <t>Isaac Clark</t>
+  </si>
+  <si>
+    <t>444 Cedar Ln.</t>
+  </si>
+  <si>
+    <t>555-8901</t>
+  </si>
+  <si>
+    <t>clark@example.edu</t>
+  </si>
+  <si>
+    <t>BIo300</t>
+  </si>
+  <si>
+    <t>S20250010</t>
+  </si>
+  <si>
+    <t>Jennifer Davis</t>
+  </si>
+  <si>
+    <t>555 Oakwood Pl.</t>
+  </si>
+  <si>
+    <t>davis@example.edu</t>
+  </si>
+  <si>
+    <t>The Renaissance: Art, Culture, and Society</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Research Interest</t>
+  </si>
+  <si>
+    <t>Office Location</t>
+  </si>
+  <si>
+    <t>Courses Offered</t>
+  </si>
+  <si>
     <t>F0001</t>
   </si>
   <si>
-    <t>Literature Basics</t>
-  </si>
-  <si>
-    <t>ENG101</t>
-  </si>
-  <si>
-    <t>Section 2</t>
-  </si>
-  <si>
-    <t>Tue/Thu 10-12 PM</t>
-  </si>
-  <si>
-    <t>12/16/2025 10:00</t>
-  </si>
-  <si>
-    <t>Room 102</t>
-  </si>
-  <si>
-    <t>Unassigned</t>
-  </si>
-  <si>
-    <t>Mon/Wed 10-12 PM</t>
-  </si>
-  <si>
-    <t>Introduction to Programming</t>
-  </si>
-  <si>
-    <t>CS201</t>
-  </si>
-  <si>
-    <t>Tue/Thu 12-2 PM</t>
-  </si>
-  <si>
-    <t>12/16/2025 12:30</t>
-  </si>
-  <si>
-    <t>Room 103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prof. Bahar Nozari </t>
-  </si>
-  <si>
-    <t>Introduction to Chemistry</t>
-  </si>
-  <si>
-    <t>CHEM200</t>
-  </si>
-  <si>
-    <t>Mon/ Thu 3-4 PM</t>
-  </si>
-  <si>
-    <t>12/14/2025 04:00</t>
-  </si>
-  <si>
-    <t>Room 201</t>
-  </si>
-  <si>
-    <t>Dr. Lucka Lucku</t>
-  </si>
-  <si>
-    <t>Mon/ Tue 5-6 PM</t>
-  </si>
-  <si>
-    <t>Section 3</t>
-  </si>
-  <si>
-    <t>Fri/ Thu 2-3 PM</t>
-  </si>
-  <si>
-    <t>Introduction to French</t>
-  </si>
-  <si>
-    <t>Tue/Thur 4:30 - 5:30 PM</t>
-  </si>
-  <si>
-    <t>12/13/2025 10:00</t>
-  </si>
-  <si>
-    <t>Room 202</t>
-  </si>
-  <si>
-    <t>Dr. Lakyn Copeland</t>
-  </si>
-  <si>
-    <t>Tue/Thur 5:30 - 6:30 PM</t>
-  </si>
-  <si>
-    <t>Water Resources</t>
-  </si>
-  <si>
-    <t>ENGG402</t>
-  </si>
-  <si>
-    <t>Mon/Fri 9:00 - 10:30</t>
-  </si>
-  <si>
-    <t>12/01/2025 09:00</t>
-  </si>
-  <si>
-    <t>Room 203</t>
-  </si>
-  <si>
-    <t>Dr. Albozr Gharabaghi</t>
-  </si>
-  <si>
-    <t>Student ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Academic Level</t>
-  </si>
-  <si>
-    <t>Current Semester</t>
-  </si>
-  <si>
-    <t>Profile Picture</t>
-  </si>
-  <si>
-    <t>Registered Subjects</t>
-  </si>
-  <si>
-    <t>Thesis Title</t>
-  </si>
-  <si>
-    <t>Progress</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>S20250001</t>
-  </si>
-  <si>
-    <t>Alice Smith</t>
-  </si>
-  <si>
-    <t>123 Maple St.</t>
-  </si>
-  <si>
-    <t>555-1234</t>
-  </si>
-  <si>
-    <t>alice@example.edu</t>
-  </si>
-  <si>
-    <t>Undergraduate</t>
-  </si>
-  <si>
-    <t>Fall 2025</t>
-  </si>
-  <si>
-    <t>custom</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>default123</t>
-  </si>
-  <si>
-    <t>S20250002</t>
-  </si>
-  <si>
-    <t>Bob Johnson</t>
-  </si>
-  <si>
-    <t>456 Oak St.</t>
-  </si>
-  <si>
-    <t>555-5678</t>
-  </si>
-  <si>
-    <t>bob@example.edu</t>
-  </si>
-  <si>
-    <t>Graduate</t>
-  </si>
-  <si>
-    <t>"The detection of oil under ice by remote mode conversion of ultrasound"</t>
-  </si>
-  <si>
-    <t>S20250003</t>
-  </si>
-  <si>
-    <t>Carol Williams</t>
-  </si>
-  <si>
-    <t>789 Pine St.</t>
-  </si>
-  <si>
-    <t>555-9012</t>
-  </si>
-  <si>
-    <t>carol@example.edu</t>
-  </si>
-  <si>
-    <t>ENGG402, HIST101</t>
-  </si>
-  <si>
-    <t>"On the economic optimality of marine reserves when fishing damages habitat"</t>
-  </si>
-  <si>
-    <t>S20250004</t>
-  </si>
-  <si>
-    <t>Lucka Racki</t>
-  </si>
-  <si>
-    <t>1767 Jane St.</t>
-  </si>
-  <si>
-    <t>439-9966</t>
-  </si>
-  <si>
-    <t>lucka@example.edu</t>
-  </si>
-  <si>
-    <t>Bio300</t>
-  </si>
-  <si>
-    <t>S20250005</t>
-  </si>
-  <si>
-    <t>David Lee</t>
-  </si>
-  <si>
-    <t>90 Elm St.</t>
-  </si>
-  <si>
-    <t>555-3456</t>
-  </si>
-  <si>
-    <t>lee@example.edu</t>
-  </si>
-  <si>
-    <t>HIST101</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>S20250006</t>
-  </si>
-  <si>
-    <t>Emily Brown</t>
-  </si>
-  <si>
-    <t>111 Oak Ave.</t>
-  </si>
-  <si>
-    <t>555-7890</t>
-  </si>
-  <si>
-    <t>brown@example.edu</t>
-  </si>
-  <si>
-    <t>Chem200</t>
-  </si>
-  <si>
-    <t>Synthesis and Characterization of Novel Catalysts</t>
-  </si>
-  <si>
-    <t>S20250007</t>
-  </si>
-  <si>
-    <t>George Smith</t>
-  </si>
-  <si>
-    <t>222 Pine Rd.</t>
-  </si>
-  <si>
-    <t>555-2345</t>
-  </si>
-  <si>
-    <t>smith@example.edu</t>
-  </si>
-  <si>
-    <t>Music102</t>
-  </si>
-  <si>
-    <t>S20250008</t>
-  </si>
-  <si>
-    <t>Helen Jones</t>
-  </si>
-  <si>
-    <t>333 Maple Dr.</t>
-  </si>
-  <si>
-    <t>555-4567</t>
-  </si>
-  <si>
-    <t>jones@example.edu</t>
-  </si>
-  <si>
-    <t>PSYCHO100, Music102, HIST101</t>
-  </si>
-  <si>
-    <t>The Effects of Stress on Cognitive Function</t>
-  </si>
-  <si>
-    <t>S20250009</t>
-  </si>
-  <si>
-    <t>Isaac Clark</t>
-  </si>
-  <si>
-    <t>444 Cedar Ln.</t>
-  </si>
-  <si>
-    <t>555-8901</t>
-  </si>
-  <si>
-    <t>clark@example.edu</t>
-  </si>
-  <si>
-    <t>BIo300</t>
-  </si>
-  <si>
-    <t>S20250010</t>
-  </si>
-  <si>
-    <t>Jennifer Davis</t>
-  </si>
-  <si>
-    <t>555 Oakwood Pl.</t>
-  </si>
-  <si>
-    <t>davis@example.edu</t>
-  </si>
-  <si>
-    <t>The Renaissance: Art, Culture, and Society</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Degree</t>
-  </si>
-  <si>
-    <t>Research Interest</t>
-  </si>
-  <si>
-    <t>Office Location</t>
-  </si>
-  <si>
-    <t>Courses Offered</t>
-  </si>
-  <si>
-    <t>Dr. Alan Turing</t>
-  </si>
-  <si>
     <t>Ph.D.</t>
   </si>
   <si>
@@ -441,9 +441,6 @@
     <t>F0002</t>
   </si>
   <si>
-    <t>Prof. Emily Brontë</t>
-  </si>
-  <si>
     <t>Master's</t>
   </si>
   <si>
@@ -589,6 +586,27 @@
   </si>
   <si>
     <t>Alice Smith, Bob Johnson, Lucka Racki, Helen Jones, David Lee</t>
+  </si>
+  <si>
+    <t>EV0001</t>
+  </si>
+  <si>
+    <t>idk</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>thorn</t>
+  </si>
+  <si>
+    <t>02/25/2025 12:59</t>
+  </si>
+  <si>
+    <t>$5</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -948,22 +966,22 @@
         <v>17</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E3" t="n" s="0">
         <v>25.0</v>
       </c>
       <c r="F3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="H3" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="I3" t="s" s="0">
         <v>21</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -977,7 +995,7 @@
         <v>17</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E4" t="n" s="0">
         <v>25.0</v>
@@ -986,13 +1004,13 @@
         <v>23</v>
       </c>
       <c r="G4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="I4" t="s" s="0">
         <v>21</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -1064,7 +1082,7 @@
         <v>31</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E7" t="n" s="0">
         <v>50.0</v>
@@ -1151,7 +1169,7 @@
         <v>17</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E10" t="n" s="0">
         <v>25.0</v>
@@ -1670,10 +1688,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>15</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>136</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>137</v>
@@ -1699,16 +1717,16 @@
         <v>140</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="D3" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="E3" t="s" s="0">
         <v>143</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>144</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>42</v>
@@ -1722,25 +1740,25 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>145</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>146</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>137</v>
       </c>
       <c r="D4" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="F4" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="G4" t="s" s="0">
         <v>149</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>150</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>72</v>
@@ -1748,19 +1766,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>43</v>
       </c>
       <c r="C5" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>143</v>
-      </c>
       <c r="E5" t="s" s="0">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>34</v>
@@ -1774,22 +1792,22 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>153</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>154</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>137</v>
       </c>
       <c r="D6" t="s" s="0">
+        <v>154</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="F6" t="s" s="0">
         <v>156</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>157</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>45</v>
@@ -1816,7 +1834,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s" s="31">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2">
@@ -1824,7 +1842,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3">
@@ -1832,7 +1850,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4">
@@ -1840,7 +1858,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5">
@@ -1848,15 +1866,15 @@
         <v>31</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>163</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>164</v>
       </c>
     </row>
     <row r="7">
@@ -1864,7 +1882,7 @@
         <v>46</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8">
@@ -1872,23 +1890,23 @@
         <v>98</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="B9" t="s" s="0">
         <v>167</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>168</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="B10" t="s" s="0">
         <v>169</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1898,7 +1916,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1906,89 +1924,118 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="32">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s" s="33">
         <v>52</v>
       </c>
       <c r="C1" t="s" s="34">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s" s="35">
         <v>7</v>
       </c>
       <c r="E1" t="s" s="36">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F1" t="s" s="37">
         <v>4</v>
       </c>
       <c r="G1" t="s" s="38">
+        <v>173</v>
+      </c>
+      <c r="H1" t="s" s="39">
         <v>174</v>
       </c>
-      <c r="H1" t="s" s="39">
+      <c r="I1" t="s" s="40">
         <v>175</v>
-      </c>
-      <c r="I1" t="s" s="40">
-        <v>176</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="D2" t="s" s="0">
         <v>179</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="E2" t="s" s="0">
         <v>180</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>181</v>
       </c>
       <c r="F2" t="n" s="0">
         <v>100.0</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>70</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>184</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s" s="0">
         <v>185</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="D3" t="s" s="0">
         <v>186</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="E3" t="s" s="0">
         <v>187</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>188</v>
       </c>
       <c r="F3" t="n" s="0">
         <v>50.0</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>70</v>
       </c>
       <c r="I3" t="s" s="0">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>190</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added profile faculty additions
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data1.xlsx
+++ b/src/main/resources/UMS_Data1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="191">
   <si>
     <t>Course Code</t>
   </si>
@@ -438,6 +438,9 @@
     <t>turing@university.edu</t>
   </si>
   <si>
+    <t>hi</t>
+  </si>
+  <si>
     <t>F0002</t>
   </si>
   <si>
@@ -564,7 +567,7 @@
     <t>Free</t>
   </si>
   <si>
-    <t>Alice Smith, Bob Johnson, Jennifer Davis, Helen Jones, S20250010</t>
+    <t>Alice Smith, Bob Johnson, Jennifer Davis, Helen Jones</t>
   </si>
   <si>
     <t>EV002</t>
@@ -1688,24 +1691,24 @@
         <v>9</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>21</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>42</v>
@@ -1719,25 +1722,25 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>137</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>72</v>
@@ -1745,19 +1748,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>43</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>34</v>
@@ -1771,22 +1774,22 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>137</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>45</v>
@@ -1813,7 +1816,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s" s="31">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2">
@@ -1821,7 +1824,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3">
@@ -1829,7 +1832,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4">
@@ -1837,7 +1840,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5">
@@ -1845,15 +1848,15 @@
         <v>31</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7">
@@ -1861,7 +1864,7 @@
         <v>46</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8">
@@ -1869,23 +1872,23 @@
         <v>98</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1903,89 +1906,89 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="32">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s" s="33">
         <v>52</v>
       </c>
       <c r="C1" t="s" s="34">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D1" t="s" s="35">
         <v>7</v>
       </c>
       <c r="E1" t="s" s="36">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F1" t="s" s="37">
         <v>4</v>
       </c>
       <c r="G1" t="s" s="38">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H1" t="s" s="39">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I1" t="s" s="40">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F2" t="n" s="0">
         <v>100.0</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>70</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F3" t="n" s="0">
         <v>50.0</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>70</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added student faculty view
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data1.xlsx
+++ b/src/main/resources/UMS_Data1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="190">
   <si>
     <t>Course Code</t>
   </si>
@@ -63,372 +63,375 @@
     <t>Room 101</t>
   </si>
   <si>
+    <t>F0001</t>
+  </si>
+  <si>
+    <t>Literature Basics</t>
+  </si>
+  <si>
+    <t>ENG101</t>
+  </si>
+  <si>
+    <t>Tue/Thu 10-12 PM</t>
+  </si>
+  <si>
+    <t>12/16/2025 10:00</t>
+  </si>
+  <si>
+    <t>Room 102</t>
+  </si>
+  <si>
+    <t>F0002</t>
+  </si>
+  <si>
+    <t>Section 2</t>
+  </si>
+  <si>
+    <t>Mon/Wed 10-12 PM</t>
+  </si>
+  <si>
+    <t>Prof. Emily Brontë</t>
+  </si>
+  <si>
+    <t>Introduction to Programming</t>
+  </si>
+  <si>
+    <t>CS201</t>
+  </si>
+  <si>
+    <t>Tue/Thu 12-2 PM</t>
+  </si>
+  <si>
+    <t>12/16/2025 12:30</t>
+  </si>
+  <si>
+    <t>Room 103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prof. Bahar Nozari </t>
+  </si>
+  <si>
+    <t>Introduction to Chemistry</t>
+  </si>
+  <si>
+    <t>CHEM200</t>
+  </si>
+  <si>
+    <t>Mon/ Thu 3-4 PM</t>
+  </si>
+  <si>
+    <t>12/14/2025 04:00</t>
+  </si>
+  <si>
+    <t>Room 201</t>
+  </si>
+  <si>
+    <t>Dr. Lucka Lucku</t>
+  </si>
+  <si>
+    <t>Mon/ Tue 5-6 PM</t>
+  </si>
+  <si>
+    <t>Section 3</t>
+  </si>
+  <si>
+    <t>Fri/ Thu 2-3 PM</t>
+  </si>
+  <si>
+    <t>Introduction to French</t>
+  </si>
+  <si>
+    <t>Tue/Thur 4:30 - 5:30 PM</t>
+  </si>
+  <si>
+    <t>12/13/2025 10:00</t>
+  </si>
+  <si>
+    <t>Room 202</t>
+  </si>
+  <si>
+    <t>Dr. Lakyn Copeland</t>
+  </si>
+  <si>
+    <t>Tue/Thur 5:30 - 6:30 PM</t>
+  </si>
+  <si>
+    <t>Water Resources</t>
+  </si>
+  <si>
+    <t>ENGG402</t>
+  </si>
+  <si>
+    <t>Mon/Fri 9:00 - 10:30</t>
+  </si>
+  <si>
+    <t>12/01/2025 09:00</t>
+  </si>
+  <si>
+    <t>Room 203</t>
+  </si>
+  <si>
+    <t>Dr. Albozr Gharabaghi</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Academic Level</t>
+  </si>
+  <si>
+    <t>Current Semester</t>
+  </si>
+  <si>
+    <t>Profile Picture</t>
+  </si>
+  <si>
+    <t>Registered Subjects</t>
+  </si>
+  <si>
+    <t>Thesis Title</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>S20250001</t>
+  </si>
+  <si>
+    <t>Alice Smith</t>
+  </si>
+  <si>
+    <t>123 Maple St.</t>
+  </si>
+  <si>
+    <t>555-1234</t>
+  </si>
+  <si>
+    <t>alice@example.edu</t>
+  </si>
+  <si>
+    <t>Undergraduate</t>
+  </si>
+  <si>
+    <t>Fall 2025</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>default123</t>
+  </si>
+  <si>
+    <t>S20250002</t>
+  </si>
+  <si>
+    <t>Bob Johnson</t>
+  </si>
+  <si>
+    <t>456 Oak St.</t>
+  </si>
+  <si>
+    <t>555-5678</t>
+  </si>
+  <si>
+    <t>bob@example.edu</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>"The detection of oil under ice by remote mode conversion of ultrasound"</t>
+  </si>
+  <si>
+    <t>S20250003</t>
+  </si>
+  <si>
+    <t>Carol Williams</t>
+  </si>
+  <si>
+    <t>789 Pine St.</t>
+  </si>
+  <si>
+    <t>555-9012</t>
+  </si>
+  <si>
+    <t>carol@example.edu</t>
+  </si>
+  <si>
+    <t>ENGG402, HIST101</t>
+  </si>
+  <si>
+    <t>"On the economic optimality of marine reserves when fishing damages habitat"</t>
+  </si>
+  <si>
+    <t>S20250004</t>
+  </si>
+  <si>
+    <t>Lucka Racki</t>
+  </si>
+  <si>
+    <t>1767 Jane St.</t>
+  </si>
+  <si>
+    <t>439-9966</t>
+  </si>
+  <si>
+    <t>lucka@example.edu</t>
+  </si>
+  <si>
+    <t>Bio300</t>
+  </si>
+  <si>
+    <t>S20250005</t>
+  </si>
+  <si>
+    <t>David Lee</t>
+  </si>
+  <si>
+    <t>90 Elm St.</t>
+  </si>
+  <si>
+    <t>555-3456</t>
+  </si>
+  <si>
+    <t>lee@example.edu</t>
+  </si>
+  <si>
+    <t>HIST101</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>S20250006</t>
+  </si>
+  <si>
+    <t>Emily Brown</t>
+  </si>
+  <si>
+    <t>111 Oak Ave.</t>
+  </si>
+  <si>
+    <t>555-7890</t>
+  </si>
+  <si>
+    <t>brown@example.edu</t>
+  </si>
+  <si>
+    <t>Chem200</t>
+  </si>
+  <si>
+    <t>Synthesis and Characterization of Novel Catalysts</t>
+  </si>
+  <si>
+    <t>S20250007</t>
+  </si>
+  <si>
+    <t>George Smith</t>
+  </si>
+  <si>
+    <t>222 Pine Rd.</t>
+  </si>
+  <si>
+    <t>555-2345</t>
+  </si>
+  <si>
+    <t>smith@example.edu</t>
+  </si>
+  <si>
+    <t>Music102</t>
+  </si>
+  <si>
+    <t>S20250008</t>
+  </si>
+  <si>
+    <t>Helen Jones</t>
+  </si>
+  <si>
+    <t>333 Maple Dr.</t>
+  </si>
+  <si>
+    <t>555-4567</t>
+  </si>
+  <si>
+    <t>jones@example.edu</t>
+  </si>
+  <si>
+    <t>PSYCHO100, Music102, HIST101</t>
+  </si>
+  <si>
+    <t>The Effects of Stress on Cognitive Function</t>
+  </si>
+  <si>
+    <t>S20250009</t>
+  </si>
+  <si>
+    <t>Isaac Clark</t>
+  </si>
+  <si>
+    <t>444 Cedar Ln.</t>
+  </si>
+  <si>
+    <t>555-8901</t>
+  </si>
+  <si>
+    <t>clark@example.edu</t>
+  </si>
+  <si>
+    <t>BIo300</t>
+  </si>
+  <si>
+    <t>S20250010</t>
+  </si>
+  <si>
+    <t>Jennifer Davis</t>
+  </si>
+  <si>
+    <t>555 Oakwood Pl.</t>
+  </si>
+  <si>
+    <t>davis@example.edu</t>
+  </si>
+  <si>
+    <t>The Renaissance: Art, Culture, and Society</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Research Interest</t>
+  </si>
+  <si>
+    <t>Office Location</t>
+  </si>
+  <si>
+    <t>Courses Offered</t>
+  </si>
+  <si>
     <t>Dr. Alan Turing</t>
   </si>
   <si>
-    <t>Literature Basics</t>
-  </si>
-  <si>
-    <t>ENG101</t>
-  </si>
-  <si>
-    <t>Tue/Thu 10-12 PM</t>
-  </si>
-  <si>
-    <t>12/16/2025 10:00</t>
-  </si>
-  <si>
-    <t>Room 102</t>
-  </si>
-  <si>
-    <t>Prof. Emily Brontë</t>
-  </si>
-  <si>
-    <t>Section 2</t>
-  </si>
-  <si>
-    <t>Mon/Wed 10-12 PM</t>
-  </si>
-  <si>
-    <t>Introduction to Programming</t>
-  </si>
-  <si>
-    <t>CS201</t>
-  </si>
-  <si>
-    <t>Tue/Thu 12-2 PM</t>
-  </si>
-  <si>
-    <t>12/16/2025 12:30</t>
-  </si>
-  <si>
-    <t>Room 103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prof. Bahar Nozari </t>
-  </si>
-  <si>
-    <t>Introduction to Chemistry</t>
-  </si>
-  <si>
-    <t>CHEM200</t>
-  </si>
-  <si>
-    <t>Mon/ Thu 3-4 PM</t>
-  </si>
-  <si>
-    <t>12/14/2025 04:00</t>
-  </si>
-  <si>
-    <t>Room 201</t>
-  </si>
-  <si>
-    <t>Dr. Lucka Lucku</t>
-  </si>
-  <si>
-    <t>Mon/ Tue 5-6 PM</t>
-  </si>
-  <si>
-    <t>Section 3</t>
-  </si>
-  <si>
-    <t>Fri/ Thu 2-3 PM</t>
-  </si>
-  <si>
-    <t>Introduction to French</t>
-  </si>
-  <si>
-    <t>Tue/Thur 4:30 - 5:30 PM</t>
-  </si>
-  <si>
-    <t>12/13/2025 10:00</t>
-  </si>
-  <si>
-    <t>Room 202</t>
-  </si>
-  <si>
-    <t>Dr. Lakyn Copeland</t>
-  </si>
-  <si>
-    <t>Tue/Thur 5:30 - 6:30 PM</t>
-  </si>
-  <si>
-    <t>Water Resources</t>
-  </si>
-  <si>
-    <t>ENGG402</t>
-  </si>
-  <si>
-    <t>Mon/Fri 9:00 - 10:30</t>
-  </si>
-  <si>
-    <t>12/01/2025 09:00</t>
-  </si>
-  <si>
-    <t>Room 203</t>
-  </si>
-  <si>
-    <t>Dr. Albozr Gharabaghi</t>
-  </si>
-  <si>
-    <t>Student ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Academic Level</t>
-  </si>
-  <si>
-    <t>Current Semester</t>
-  </si>
-  <si>
-    <t>Profile Picture</t>
-  </si>
-  <si>
-    <t>Registered Subjects</t>
-  </si>
-  <si>
-    <t>Thesis Title</t>
-  </si>
-  <si>
-    <t>Progress</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>S20250001</t>
-  </si>
-  <si>
-    <t>Alice Smith</t>
-  </si>
-  <si>
-    <t>123 Maple St.</t>
-  </si>
-  <si>
-    <t>555-1234</t>
-  </si>
-  <si>
-    <t>alice@example.edu</t>
-  </si>
-  <si>
-    <t>Undergraduate</t>
-  </si>
-  <si>
-    <t>Fall 2025</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>default123</t>
-  </si>
-  <si>
-    <t>S20250002</t>
-  </si>
-  <si>
-    <t>Bob Johnson</t>
-  </si>
-  <si>
-    <t>456 Oak St.</t>
-  </si>
-  <si>
-    <t>555-5678</t>
-  </si>
-  <si>
-    <t>bob@example.edu</t>
-  </si>
-  <si>
-    <t>Graduate</t>
-  </si>
-  <si>
-    <t>"The detection of oil under ice by remote mode conversion of ultrasound"</t>
-  </si>
-  <si>
-    <t>S20250003</t>
-  </si>
-  <si>
-    <t>Carol Williams</t>
-  </si>
-  <si>
-    <t>789 Pine St.</t>
-  </si>
-  <si>
-    <t>555-9012</t>
-  </si>
-  <si>
-    <t>carol@example.edu</t>
-  </si>
-  <si>
-    <t>ENGG402, HIST101</t>
-  </si>
-  <si>
-    <t>"On the economic optimality of marine reserves when fishing damages habitat"</t>
-  </si>
-  <si>
-    <t>S20250004</t>
-  </si>
-  <si>
-    <t>Lucka Racki</t>
-  </si>
-  <si>
-    <t>1767 Jane St.</t>
-  </si>
-  <si>
-    <t>439-9966</t>
-  </si>
-  <si>
-    <t>lucka@example.edu</t>
-  </si>
-  <si>
-    <t>Bio300</t>
-  </si>
-  <si>
-    <t>S20250005</t>
-  </si>
-  <si>
-    <t>David Lee</t>
-  </si>
-  <si>
-    <t>90 Elm St.</t>
-  </si>
-  <si>
-    <t>555-3456</t>
-  </si>
-  <si>
-    <t>lee@example.edu</t>
-  </si>
-  <si>
-    <t>HIST101</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>S20250006</t>
-  </si>
-  <si>
-    <t>Emily Brown</t>
-  </si>
-  <si>
-    <t>111 Oak Ave.</t>
-  </si>
-  <si>
-    <t>555-7890</t>
-  </si>
-  <si>
-    <t>brown@example.edu</t>
-  </si>
-  <si>
-    <t>Chem200</t>
-  </si>
-  <si>
-    <t>Synthesis and Characterization of Novel Catalysts</t>
-  </si>
-  <si>
-    <t>S20250007</t>
-  </si>
-  <si>
-    <t>George Smith</t>
-  </si>
-  <si>
-    <t>222 Pine Rd.</t>
-  </si>
-  <si>
-    <t>555-2345</t>
-  </si>
-  <si>
-    <t>smith@example.edu</t>
-  </si>
-  <si>
-    <t>Music102</t>
-  </si>
-  <si>
-    <t>S20250008</t>
-  </si>
-  <si>
-    <t>Helen Jones</t>
-  </si>
-  <si>
-    <t>333 Maple Dr.</t>
-  </si>
-  <si>
-    <t>555-4567</t>
-  </si>
-  <si>
-    <t>jones@example.edu</t>
-  </si>
-  <si>
-    <t>PSYCHO100, Music102, HIST101</t>
-  </si>
-  <si>
-    <t>The Effects of Stress on Cognitive Function</t>
-  </si>
-  <si>
-    <t>S20250009</t>
-  </si>
-  <si>
-    <t>Isaac Clark</t>
-  </si>
-  <si>
-    <t>444 Cedar Ln.</t>
-  </si>
-  <si>
-    <t>555-8901</t>
-  </si>
-  <si>
-    <t>clark@example.edu</t>
-  </si>
-  <si>
-    <t>BIo300</t>
-  </si>
-  <si>
-    <t>S20250010</t>
-  </si>
-  <si>
-    <t>Jennifer Davis</t>
-  </si>
-  <si>
-    <t>555 Oakwood Pl.</t>
-  </si>
-  <si>
-    <t>davis@example.edu</t>
-  </si>
-  <si>
-    <t>The Renaissance: Art, Culture, and Society</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Degree</t>
-  </si>
-  <si>
-    <t>Research Interest</t>
-  </si>
-  <si>
-    <t>Office Location</t>
-  </si>
-  <si>
-    <t>Courses Offered</t>
-  </si>
-  <si>
-    <t>F0001</t>
-  </si>
-  <si>
     <t>Ph.D.</t>
   </si>
   <si>
@@ -438,9 +441,6 @@
     <t>turing@university.edu</t>
   </si>
   <si>
-    <t>F0002</t>
-  </si>
-  <si>
     <t>Master's</t>
   </si>
   <si>
@@ -562,9 +562,6 @@
   </si>
   <si>
     <t>Free</t>
-  </si>
-  <si>
-    <t>file:/C:/Users/adria/OneDrive/Pictures/Screenshots%201/Screenshot%202025-04-02%20184051.png</t>
   </si>
   <si>
     <t>Helen Jones, Jennifer Davis, Alice Smith, Bob Johnson</t>
@@ -992,7 +989,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -1000,10 +997,10 @@
         <v>3.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>11</v>
@@ -1012,16 +1009,16 @@
         <v>42.0</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
@@ -1029,10 +1026,10 @@
         <v>4.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>11</v>
@@ -1041,16 +1038,16 @@
         <v>50.0</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
@@ -1058,10 +1055,10 @@
         <v>4.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>22</v>
@@ -1070,16 +1067,16 @@
         <v>50.0</v>
       </c>
       <c r="F7" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s" s="0">
         <v>36</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>35</v>
       </c>
     </row>
     <row r="8">
@@ -1087,28 +1084,28 @@
         <v>4.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" t="n" s="0">
         <v>50.0</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
@@ -1116,7 +1113,7 @@
         <v>5.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>17</v>
@@ -1128,16 +1125,16 @@
         <v>25.0</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
@@ -1145,7 +1142,7 @@
         <v>5.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>17</v>
@@ -1157,16 +1154,16 @@
         <v>25.0</v>
       </c>
       <c r="F10" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s" s="0">
         <v>44</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="I10" t="s" s="0">
-        <v>43</v>
       </c>
     </row>
     <row r="11">
@@ -1174,10 +1171,10 @@
         <v>6.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s" s="0">
         <v>11</v>
@@ -1186,16 +1183,16 @@
         <v>50.0</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1213,420 +1210,420 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="10">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s" s="11">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s" s="12">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s" s="13">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s" s="14">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s" s="15">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s" s="17">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I1" t="s" s="18">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J1" t="s" s="19">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K1" t="s" s="20">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L1" t="s" s="21">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K2" t="n" s="0">
         <v>0.4</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K3" t="n" s="0">
         <v>0.5</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K4" t="n" s="0">
         <v>0.5</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K5" t="n" s="0">
         <v>0.6</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K6" t="n" s="0">
         <v>0.5</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K7" t="n" s="0">
         <v>0.5</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K8" t="n" s="0">
         <v>0.4</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K9" t="n" s="0">
         <v>0.5</v>
       </c>
       <c r="L9" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J10" t="s" s="0">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K10" t="n" s="0">
         <v>0.5</v>
       </c>
       <c r="L10" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J11" t="s" s="0">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K11" t="n" s="0">
         <v>0.2</v>
       </c>
       <c r="L11" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1644,65 +1641,65 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="22">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s" s="23">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s" s="24">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s" s="25">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E1" t="s" s="26">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s" s="27">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s" s="28">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s" s="29">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>140</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>141</v>
@@ -1714,16 +1711,16 @@
         <v>143</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
@@ -1734,7 +1731,7 @@
         <v>145</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>146</v>
@@ -1749,10 +1746,10 @@
         <v>149</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
@@ -1760,7 +1757,7 @@
         <v>150</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>141</v>
@@ -1772,16 +1769,16 @@
         <v>151</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6">
@@ -1792,7 +1789,7 @@
         <v>153</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>154</v>
@@ -1804,13 +1801,13 @@
         <v>156</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1852,7 +1849,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>160</v>
@@ -1860,7 +1857,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>161</v>
@@ -1876,7 +1873,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>164</v>
@@ -1884,7 +1881,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>165</v>
@@ -1924,7 +1921,7 @@
         <v>170</v>
       </c>
       <c r="B1" t="s" s="33">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s" s="34">
         <v>171</v>
@@ -1971,39 +1968,39 @@
         <v>181</v>
       </c>
       <c r="H2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s" s="0">
         <v>182</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>184</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s" s="0">
         <v>185</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="D3" t="s" s="0">
         <v>186</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="E3" t="s" s="0">
         <v>187</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>188</v>
       </c>
       <c r="F3" t="n" s="0">
         <v>50.0</v>
       </c>
       <c r="G3" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s" s="0">
         <v>189</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted unused files and packages
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data1.xlsx
+++ b/src/main/resources/UMS_Data1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="197">
   <si>
     <t>Course Code</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Room 103</t>
   </si>
   <si>
-    <t>Prof. Bahar Nozari</t>
-  </si>
-  <si>
     <t>Introduction to Chemistry</t>
   </si>
   <si>
@@ -234,63 +231,72 @@
     <t>default</t>
   </si>
   <si>
+    <t>ENG101, MATH001</t>
+  </si>
+  <si>
     <t>_</t>
   </si>
   <si>
     <t>40.0%</t>
   </si>
   <si>
+    <t>default1234</t>
+  </si>
+  <si>
+    <t>S20250002</t>
+  </si>
+  <si>
+    <t>Bob Johnson</t>
+  </si>
+  <si>
+    <t>456 Oak St.</t>
+  </si>
+  <si>
+    <t>555-5678</t>
+  </si>
+  <si>
+    <t>bob@example.edu</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>CS201, ENG101</t>
+  </si>
+  <si>
+    <t>"The detection of oil under ice by remote mode conversion of ultrasound"</t>
+  </si>
+  <si>
+    <t>50.0%</t>
+  </si>
+  <si>
+    <t>default123</t>
+  </si>
+  <si>
+    <t>S20250003</t>
+  </si>
+  <si>
+    <t>Carol Williams</t>
+  </si>
+  <si>
+    <t>789 Pine St.</t>
+  </si>
+  <si>
+    <t>555-9012</t>
+  </si>
+  <si>
+    <t>carol@example.edu</t>
+  </si>
+  <si>
+    <t>ENGG402, HIST101</t>
+  </si>
+  <si>
+    <t>"On the economic optimality of marine reserves when fishing damages habitat"</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>S20250002</t>
-  </si>
-  <si>
-    <t>Bob Johnson</t>
-  </si>
-  <si>
-    <t>456 Oak St.</t>
-  </si>
-  <si>
-    <t>555-5678</t>
-  </si>
-  <si>
-    <t>bob@example.edu</t>
-  </si>
-  <si>
-    <t>Graduate</t>
-  </si>
-  <si>
-    <t>"The detection of oil under ice by remote mode conversion of ultrasound"</t>
-  </si>
-  <si>
-    <t>50.0%</t>
-  </si>
-  <si>
-    <t>default123</t>
-  </si>
-  <si>
-    <t>S20250003</t>
-  </si>
-  <si>
-    <t>Carol Williams</t>
-  </si>
-  <si>
-    <t>789 Pine St.</t>
-  </si>
-  <si>
-    <t>555-9012</t>
-  </si>
-  <si>
-    <t>carol@example.edu</t>
-  </si>
-  <si>
-    <t>ENGG402, HIST101</t>
-  </si>
-  <si>
-    <t>"On the economic optimality of marine reserves when fishing damages habitat"</t>
-  </si>
-  <si>
     <t>S20250004</t>
   </si>
   <si>
@@ -456,6 +462,9 @@
     <t>turing@university.edu</t>
   </si>
   <si>
+    <t>Calculus I, Introduction to Programming</t>
+  </si>
+  <si>
     <t>F0002</t>
   </si>
   <si>
@@ -579,7 +588,7 @@
     <t>Free</t>
   </si>
   <si>
-    <t>Helen Jones, Jennifer Davis, Alice Smith, Bob Johnson</t>
+    <t>Helen Jones, Jennifer Davis, Alice Smith, Bob Johnson, David Lee</t>
   </si>
   <si>
     <t>EV002</t>
@@ -940,7 +949,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>30.0</v>
+        <v>1.0</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>12</v>
@@ -1039,7 +1048,7 @@
         <v>28</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -1047,10 +1056,10 @@
         <v>4.0</v>
       </c>
       <c r="B6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>30</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>31</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>11</v>
@@ -1059,16 +1068,16 @@
         <v>50.0</v>
       </c>
       <c r="F6" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="G6" t="s" s="0">
+      <c r="H6" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="H6" t="s" s="0">
+      <c r="I6" t="s" s="0">
         <v>34</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -1076,10 +1085,10 @@
         <v>4.0</v>
       </c>
       <c r="B7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>30</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>31</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>22</v>
@@ -1088,16 +1097,16 @@
         <v>50.0</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="H7" t="s" s="0">
+      <c r="I7" t="s" s="0">
         <v>34</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>35</v>
       </c>
     </row>
     <row r="8">
@@ -1105,28 +1114,28 @@
         <v>4.0</v>
       </c>
       <c r="B8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="C8" t="s" s="0">
-        <v>31</v>
-      </c>
       <c r="D8" t="s" s="0">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" t="n" s="0">
         <v>50.0</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="H8" t="s" s="0">
+      <c r="I8" t="s" s="0">
         <v>34</v>
-      </c>
-      <c r="I8" t="s" s="0">
-        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -1134,7 +1143,7 @@
         <v>5.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>17</v>
@@ -1146,16 +1155,16 @@
         <v>25.0</v>
       </c>
       <c r="F9" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="G9" t="s" s="0">
+      <c r="H9" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="H9" t="s" s="0">
+      <c r="I9" t="s" s="0">
         <v>42</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>43</v>
       </c>
     </row>
     <row r="10">
@@ -1163,7 +1172,7 @@
         <v>5.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>17</v>
@@ -1175,16 +1184,16 @@
         <v>25.0</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="H10" t="s" s="0">
+      <c r="I10" t="s" s="0">
         <v>42</v>
-      </c>
-      <c r="I10" t="s" s="0">
-        <v>43</v>
       </c>
     </row>
     <row r="11">
@@ -1192,10 +1201,10 @@
         <v>6.0</v>
       </c>
       <c r="B11" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s" s="0">
         <v>45</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>46</v>
       </c>
       <c r="D11" t="s" s="0">
         <v>11</v>
@@ -1204,16 +1213,16 @@
         <v>50.0</v>
       </c>
       <c r="F11" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G11" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="G11" t="s" s="0">
+      <c r="H11" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="H11" t="s" s="0">
+      <c r="I11" t="s" s="0">
         <v>49</v>
-      </c>
-      <c r="I11" t="s" s="0">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1231,72 +1240,72 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="10">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s" s="11">
         <v>51</v>
       </c>
-      <c r="B1" t="s" s="11">
+      <c r="C1" t="s" s="12">
         <v>52</v>
       </c>
-      <c r="C1" t="s" s="12">
+      <c r="D1" t="s" s="13">
         <v>53</v>
       </c>
-      <c r="D1" t="s" s="13">
+      <c r="E1" t="s" s="14">
         <v>54</v>
       </c>
-      <c r="E1" t="s" s="14">
+      <c r="F1" t="s" s="15">
         <v>55</v>
       </c>
-      <c r="F1" t="s" s="15">
+      <c r="G1" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="G1" t="s" s="16">
+      <c r="H1" t="s" s="17">
         <v>57</v>
       </c>
-      <c r="H1" t="s" s="17">
+      <c r="I1" t="s" s="18">
         <v>58</v>
       </c>
-      <c r="I1" t="s" s="18">
+      <c r="J1" t="s" s="19">
         <v>59</v>
       </c>
-      <c r="J1" t="s" s="19">
+      <c r="K1" t="s" s="20">
         <v>60</v>
       </c>
-      <c r="K1" t="s" s="20">
+      <c r="L1" t="s" s="21">
         <v>61</v>
       </c>
-      <c r="L1" t="s" s="21">
+      <c r="M1" t="s" s="22">
         <v>62</v>
-      </c>
-      <c r="M1" t="s" s="22">
-        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="D2" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="E2" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="F2" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="G2" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="H2" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="I2" t="s" s="0">
         <v>71</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>17</v>
       </c>
       <c r="J2" t="s" s="0">
         <v>72</v>
@@ -1305,10 +1314,10 @@
         <v>73</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>74</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -1331,353 +1340,353 @@
         <v>80</v>
       </c>
       <c r="G3" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H3" t="s" s="0">
-        <v>71</v>
-      </c>
       <c r="I3" t="s" s="0">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>74</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>80</v>
       </c>
       <c r="G4" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H4" t="s" s="0">
-        <v>71</v>
-      </c>
       <c r="I4" t="s" s="0">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="G5" t="s" s="0">
+      <c r="H5" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H5" t="s" s="0">
-        <v>71</v>
-      </c>
       <c r="I5" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J5" t="s" s="0">
         <v>72</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F6" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="G6" t="s" s="0">
+      <c r="H6" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H6" t="s" s="0">
-        <v>71</v>
-      </c>
       <c r="I6" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M6" t="s" s="0">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F7" t="s" s="0">
         <v>80</v>
       </c>
       <c r="G7" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H7" t="s" s="0">
-        <v>71</v>
-      </c>
       <c r="I7" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M7" t="s" s="0">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F8" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="G8" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="G8" t="s" s="0">
+      <c r="H8" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H8" t="s" s="0">
-        <v>71</v>
-      </c>
       <c r="I8" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K8" t="s" s="0">
         <v>73</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M8" t="s" s="0">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F9" t="s" s="0">
         <v>80</v>
       </c>
       <c r="G9" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H9" t="s" s="0">
-        <v>71</v>
-      </c>
       <c r="I9" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K9" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L9" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M9" t="s" s="0">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F10" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="G10" t="s" s="0">
+      <c r="H10" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H10" t="s" s="0">
-        <v>71</v>
-      </c>
       <c r="I10" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J10" t="s" s="0">
         <v>72</v>
       </c>
       <c r="K10" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L10" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M10" t="s" s="0">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>80</v>
       </c>
       <c r="G11" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H11" t="s" s="0">
-        <v>71</v>
-      </c>
       <c r="I11" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J11" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K11" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L11" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M11" t="s" s="0">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1695,173 +1704,173 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="23">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s" s="24">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s" s="25">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s" s="26">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E1" t="s" s="27">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s" s="28">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s" s="29">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H1" t="s" s="30">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>15</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>21</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1882,7 +1891,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s" s="32">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2">
@@ -1890,7 +1899,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3">
@@ -1898,7 +1907,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4">
@@ -1906,55 +1915,55 @@
         <v>25</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1972,45 +1981,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="33">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s" s="34">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s" s="35">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D1" t="s" s="36">
         <v>7</v>
       </c>
       <c r="E1" t="s" s="37">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F1" t="s" s="38">
         <v>4</v>
       </c>
       <c r="G1" t="s" s="39">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H1" t="s" s="40">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I1" t="s" s="41">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E2" t="n" s="42">
         <v>45901.416666666664</v>
@@ -2019,27 +2028,27 @@
         <v>100.0</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E3" t="n" s="42">
         <v>45935.583333333336</v>
@@ -2048,13 +2057,13 @@
         <v>50.0</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>